<commit_message>
remove hardcoded url, getting data for specified model, creating new sheet if sheet fo this model doesnt exist
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -15,14 +15,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t xml:space="preserve">2001 </t>
   </si>
   <si>
+    <t xml:space="preserve">2002 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2003 </t>
+  </si>
+  <si>
     <t xml:space="preserve">2005 </t>
   </si>
   <si>
+    <t xml:space="preserve">2006 </t>
+  </si>
+  <si>
     <t xml:space="preserve">2007 </t>
   </si>
   <si>
@@ -32,6 +41,9 @@
     <t xml:space="preserve">2009 </t>
   </si>
   <si>
+    <t xml:space="preserve">2010 </t>
+  </si>
+  <si>
     <t xml:space="preserve">2011 </t>
   </si>
   <si>
@@ -51,6 +63,9 @@
   </si>
   <si>
     <t xml:space="preserve">2017 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018 </t>
   </si>
 </sst>
 </file>
@@ -114,12 +129,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>skoda_octavia!$A$1:$A$12</f>
+              <f>skoda_octavia!$A$1:$A$17</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>skoda_octavia!$B$1:$B$12</f>
+              <f>skoda_octavia!$B$1:$B$17</f>
             </numRef>
           </val>
         </ser>
@@ -133,12 +148,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>skoda_octavia!$A$1:$A$12</f>
+              <f>skoda_octavia!$A$1:$A$17</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>skoda_octavia!$C$1:$C$12</f>
+              <f>skoda_octavia!$C$1:$C$17</f>
             </numRef>
           </val>
         </ser>
@@ -514,7 +529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C13"/>
+  <dimension ref="A2:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
       <selection activeCell="A2" sqref="A2:C46"/>
@@ -527,10 +542,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>198345</v>
+        <v>175000</v>
       </c>
       <c r="C2" t="n">
-        <v>198345</v>
+        <v>178028.3333333333</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -538,10 +553,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>143794</v>
+        <v>198000</v>
       </c>
       <c r="C3" t="n">
-        <v>176414.3333333333</v>
+        <v>198000</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -549,10 +564,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>198000</v>
+        <v>145189</v>
       </c>
       <c r="C4" t="n">
-        <v>208333.3333333333</v>
+        <v>145189</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -560,10 +575,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>132745</v>
+        <v>143794</v>
       </c>
       <c r="C5" t="n">
-        <v>137882.6666666667</v>
+        <v>176414.3333333333</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -571,10 +586,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>142251</v>
+        <v>197000</v>
       </c>
       <c r="C6" t="n">
-        <v>142251</v>
+        <v>192637.6666666667</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -582,10 +597,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>169000</v>
+        <v>198000</v>
       </c>
       <c r="C7" t="n">
-        <v>165300</v>
+        <v>208333.3333333333</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -593,10 +608,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>101625</v>
+        <v>181322.5</v>
       </c>
       <c r="C8" t="n">
-        <v>113290.6666666667</v>
+        <v>183912</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -604,10 +619,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>125750</v>
+        <v>136125.5</v>
       </c>
       <c r="C9" t="n">
-        <v>161417.75</v>
+        <v>140462.25</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -615,10 +630,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>150507.5</v>
+        <v>102317</v>
       </c>
       <c r="C10" t="n">
-        <v>142811.8333333333</v>
+        <v>115111.3333333333</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -626,10 +641,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>179000</v>
+        <v>185500</v>
       </c>
       <c r="C11" t="n">
-        <v>179000</v>
+        <v>174475</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -637,10 +652,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>27200</v>
+        <v>118167.5</v>
       </c>
       <c r="C12" t="n">
-        <v>27200</v>
+        <v>118387.375</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -648,10 +663,65 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>5</v>
+        <v>130000</v>
       </c>
       <c r="C13" t="n">
-        <v>10335.33333333333</v>
+        <v>132304.9090909091</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>143057.5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>140696.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>82000</v>
+      </c>
+      <c r="C15" t="n">
+        <v>105453</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>27200</v>
+      </c>
+      <c r="C16" t="n">
+        <v>27515.28571428571</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2584.916666666667</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>